<commit_message>
merged two excel files
</commit_message>
<xml_diff>
--- a/personality_result.xlsx
+++ b/personality_result.xlsx
@@ -693,28 +693,28 @@
         <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
         <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O2" t="n">
         <v>1</v>
@@ -726,13 +726,13 @@
         <v>1</v>
       </c>
       <c r="R2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="S2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U2" t="n">
         <v>1</v>
@@ -765,10 +765,10 @@
         <v>1</v>
       </c>
       <c r="AE2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AF2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AG2" t="n">
         <v>1</v>
@@ -777,7 +777,7 @@
         <v>1</v>
       </c>
       <c r="AI2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ2" t="n">
         <v>1</v>
@@ -789,7 +789,7 @@
         <v>1</v>
       </c>
       <c r="AM2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AN2" t="n">
         <v>1</v>
@@ -813,13 +813,13 @@
         <v>1</v>
       </c>
       <c r="AU2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AV2" t="n">
         <v>2</v>
       </c>
       <c r="AW2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX2" t="n">
         <v>2</v>

</xml_diff>